<commit_message>
Dorada troškovnika (izmjena faze dizajniranja, korekcija cijena)
</commit_message>
<xml_diff>
--- a/Documentation/Troškovnik/WareHome - troškovnik.xlsx
+++ b/Documentation/Troškovnik/WareHome - troškovnik.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e135d290de4d23d1/Škola/6. semestar/Programsko inženjerstvo/Projekt/Troškovnik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e135d290de4d23d1/Škola/6. semestar/Programsko inženjerstvo/Projekt/pi21-atkalcec-khabdija-kstrucic/Documentation/Troškovnik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="489" documentId="8_{07DCF27A-1A62-4C3D-9CFC-A6CDF19A4204}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D305E450-05F5-4475-A16F-1BB2DA2E5C62}"/>
+  <xr:revisionPtr revIDLastSave="537" documentId="8_{07DCF27A-1A62-4C3D-9CFC-A6CDF19A4204}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB4696DB-8920-415C-895F-E89DF38538CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D96EACF-807A-41D4-A723-808F9051739A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7D96EACF-807A-41D4-A723-808F9051739A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Staro" sheetId="1" r:id="rId1"/>
+    <sheet name="Novo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>STAVKA</t>
   </si>
@@ -163,6 +164,48 @@
   </si>
   <si>
     <t>IMPLEMENTACIJA</t>
+  </si>
+  <si>
+    <t>Izrada modela podataka</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije prijave u aplikaciju</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije upisa namirnica</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije popisa namirnica</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije spremanja u PDF</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije rasporeda kupovine</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije liste za kupovinu</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije uređivanja liste za kupovinu</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije predviđanja potrošnje</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije odabira ispisa liste</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije ispisa liste za kupovinu</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije email podsjetnika</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije domaćinstva</t>
+  </si>
+  <si>
+    <t>Dizajn funkcije prijave problema</t>
   </si>
 </sst>
 </file>
@@ -945,7 +988,7 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1575,4 +1618,760 @@
     <ignoredError sqref="C6:D6 C14:D14 C32:D32 C36:D36 C2" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C5CCFF-BF09-4B7C-AD21-B56BBAF80305}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="39">
+        <f>SUM(B3:B5)</f>
+        <v>10</v>
+      </c>
+      <c r="C2" s="40">
+        <f>D2/B2</f>
+        <v>200</v>
+      </c>
+      <c r="D2" s="55">
+        <f>SUM(D3:D5)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="C3" s="41">
+        <v>200</v>
+      </c>
+      <c r="D3" s="56">
+        <f>B3*C3</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="41">
+        <v>200</v>
+      </c>
+      <c r="D4" s="56">
+        <f>B4*C4</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="21">
+        <v>5</v>
+      </c>
+      <c r="C5" s="42">
+        <v>200</v>
+      </c>
+      <c r="D5" s="57">
+        <f>B5*C5</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="37">
+        <f>SUM(B7:B21)</f>
+        <v>35.5</v>
+      </c>
+      <c r="C6" s="43">
+        <f>D6/B6</f>
+        <v>200</v>
+      </c>
+      <c r="D6" s="58">
+        <f>SUM(D7:D21)</f>
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="44">
+        <v>200</v>
+      </c>
+      <c r="D7" s="59">
+        <f>B7*C7</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="22">
+        <v>2</v>
+      </c>
+      <c r="C8" s="44">
+        <v>200</v>
+      </c>
+      <c r="D8" s="59">
+        <f t="shared" ref="D8:D21" si="0">B8*C8</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="22">
+        <v>2</v>
+      </c>
+      <c r="C9" s="44">
+        <v>200</v>
+      </c>
+      <c r="D9" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="22">
+        <v>2</v>
+      </c>
+      <c r="C10" s="44">
+        <v>200</v>
+      </c>
+      <c r="D10" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="22">
+        <v>2</v>
+      </c>
+      <c r="C11" s="44">
+        <v>200</v>
+      </c>
+      <c r="D11" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="22">
+        <v>2</v>
+      </c>
+      <c r="C12" s="44">
+        <v>200</v>
+      </c>
+      <c r="D12" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="22">
+        <v>2</v>
+      </c>
+      <c r="C13" s="44">
+        <v>200</v>
+      </c>
+      <c r="D13" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="22">
+        <v>2</v>
+      </c>
+      <c r="C14" s="44">
+        <v>200</v>
+      </c>
+      <c r="D14" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="22">
+        <v>2</v>
+      </c>
+      <c r="C15" s="44">
+        <v>200</v>
+      </c>
+      <c r="D15" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="22">
+        <v>2</v>
+      </c>
+      <c r="C16" s="44">
+        <v>200</v>
+      </c>
+      <c r="D16" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="22">
+        <v>2</v>
+      </c>
+      <c r="C17" s="44">
+        <v>200</v>
+      </c>
+      <c r="D17" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="22">
+        <v>2</v>
+      </c>
+      <c r="C18" s="44">
+        <v>200</v>
+      </c>
+      <c r="D18" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="22">
+        <v>2</v>
+      </c>
+      <c r="C19" s="44">
+        <v>200</v>
+      </c>
+      <c r="D19" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="22">
+        <v>2</v>
+      </c>
+      <c r="C20" s="44">
+        <v>200</v>
+      </c>
+      <c r="D20" s="59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="23">
+        <v>8</v>
+      </c>
+      <c r="C21" s="45">
+        <v>200</v>
+      </c>
+      <c r="D21" s="60">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="35">
+        <f>SUM(B23:B39)</f>
+        <v>57</v>
+      </c>
+      <c r="C22" s="46">
+        <f>D22/B22</f>
+        <v>305.26315789473682</v>
+      </c>
+      <c r="D22" s="61">
+        <f>SUM(D23:D39)</f>
+        <v>17400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="24">
+        <v>3</v>
+      </c>
+      <c r="C23" s="47">
+        <v>400</v>
+      </c>
+      <c r="D23" s="62">
+        <f>B23*C23</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="47">
+        <v>300</v>
+      </c>
+      <c r="D24" s="62">
+        <f t="shared" ref="D24:D39" si="1">B24*C24</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="24">
+        <v>2</v>
+      </c>
+      <c r="C25" s="47">
+        <v>300</v>
+      </c>
+      <c r="D25" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="24">
+        <v>2</v>
+      </c>
+      <c r="C26" s="47">
+        <v>300</v>
+      </c>
+      <c r="D26" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="24">
+        <v>2</v>
+      </c>
+      <c r="C27" s="47">
+        <v>300</v>
+      </c>
+      <c r="D27" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="24">
+        <v>2</v>
+      </c>
+      <c r="C28" s="47">
+        <v>300</v>
+      </c>
+      <c r="D28" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="24">
+        <v>3</v>
+      </c>
+      <c r="C29" s="47">
+        <v>300</v>
+      </c>
+      <c r="D29" s="62">
+        <f>B29*C29</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="24">
+        <v>2</v>
+      </c>
+      <c r="C30" s="47">
+        <v>300</v>
+      </c>
+      <c r="D30" s="62">
+        <f>B30*C30</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="24">
+        <v>5</v>
+      </c>
+      <c r="C31" s="47">
+        <v>400</v>
+      </c>
+      <c r="D31" s="62">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="24">
+        <v>2</v>
+      </c>
+      <c r="C32" s="47">
+        <v>300</v>
+      </c>
+      <c r="D32" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="24">
+        <v>3</v>
+      </c>
+      <c r="C33" s="47">
+        <v>300</v>
+      </c>
+      <c r="D33" s="62">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="24">
+        <v>5</v>
+      </c>
+      <c r="C34" s="47">
+        <v>400</v>
+      </c>
+      <c r="D34" s="62">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="24">
+        <v>2</v>
+      </c>
+      <c r="C35" s="47">
+        <v>300</v>
+      </c>
+      <c r="D35" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="24">
+        <v>2</v>
+      </c>
+      <c r="C36" s="47">
+        <v>300</v>
+      </c>
+      <c r="D36" s="62">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="24">
+        <v>4</v>
+      </c>
+      <c r="C37" s="47">
+        <v>300</v>
+      </c>
+      <c r="D37" s="62">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="24">
+        <v>6</v>
+      </c>
+      <c r="C38" s="47">
+        <v>300</v>
+      </c>
+      <c r="D38" s="62">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="25">
+        <v>10</v>
+      </c>
+      <c r="C39" s="48">
+        <v>200</v>
+      </c>
+      <c r="D39" s="63">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="33">
+        <f>SUM(B41:B43)</f>
+        <v>17.5</v>
+      </c>
+      <c r="C40" s="49">
+        <f>D40/B40</f>
+        <v>257.14285714285717</v>
+      </c>
+      <c r="D40" s="64">
+        <f>SUM(D41:D43)</f>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="C41" s="50">
+        <v>200</v>
+      </c>
+      <c r="D41" s="65">
+        <f>B41*C41</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="26">
+        <v>5</v>
+      </c>
+      <c r="C42" s="50">
+        <v>220</v>
+      </c>
+      <c r="D42" s="65">
+        <f>B42*C42</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="27">
+        <v>10</v>
+      </c>
+      <c r="C43" s="51">
+        <v>290</v>
+      </c>
+      <c r="D43" s="66">
+        <f>B43*C43</f>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="31">
+        <f>SUM(B45:B47)</f>
+        <v>30</v>
+      </c>
+      <c r="C44" s="52">
+        <f>D44/B44</f>
+        <v>300</v>
+      </c>
+      <c r="D44" s="67">
+        <f>SUM(D45:D47)</f>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="28">
+        <v>10</v>
+      </c>
+      <c r="C45" s="53">
+        <v>350</v>
+      </c>
+      <c r="D45" s="68">
+        <f>B45*C45</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="28">
+        <v>10</v>
+      </c>
+      <c r="C46" s="53">
+        <v>350</v>
+      </c>
+      <c r="D46" s="68">
+        <f t="shared" ref="D46:D47" si="2">B46*C46</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="29">
+        <v>10</v>
+      </c>
+      <c r="C47" s="54">
+        <v>200</v>
+      </c>
+      <c r="D47" s="69">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="72">
+        <f>SUM(B2,B6,B22,B40,B44)</f>
+        <v>150</v>
+      </c>
+      <c r="C48" s="73">
+        <f>D48/B48</f>
+        <v>266.66666666666669</v>
+      </c>
+      <c r="D48" s="70">
+        <f>SUM(D44,D40,D22,D6,D2)</f>
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>